<commit_message>
3D plots for 10mm BPA
</commit_message>
<xml_diff>
--- a/DataCollection/BPAparameters_normalized.xlsx
+++ b/DataCollection/BPAparameters_normalized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E70A38-43DF-49D8-AC56-6E14A4FEACFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528F09B8-BFE1-43B1-88E2-4A31BC7CF29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8A3A5EB0-BE78-4EAA-84C9-DD014A3A2FAA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8A3A5EB0-BE78-4EAA-84C9-DD014A3A2FAA}"/>
   </bookViews>
   <sheets>
     <sheet name="10mm" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Cut length</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Max strain (%)</t>
+  </si>
+  <si>
+    <t>Relative strain</t>
   </si>
 </sst>
 </file>
@@ -644,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F760E8-92D5-4163-ADDE-07026F3D9A53}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,9 +664,10 @@
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -694,8 +698,11 @@
       <c r="J1" s="23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>13.7</v>
       </c>
@@ -725,15 +732,19 @@
         <v>16.666666666666664</v>
       </c>
       <c r="I2" s="1">
-        <f>(B2-D2)/B2</f>
+        <f t="shared" ref="I2:I20" si="0">(B2-D2)/B2</f>
         <v>0</v>
       </c>
       <c r="J2" s="6">
         <f>I2*100</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="24">
+        <f>J2/H2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>13.7</v>
       </c>
@@ -747,31 +758,35 @@
         <v>11.6</v>
       </c>
       <c r="E3" s="18">
-        <f t="shared" ref="E3:E20" si="0">B3-D3</f>
+        <f t="shared" ref="E3:E20" si="1">B3-D3</f>
         <v>0.40000000000000036</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F20" si="1">D3/B3</f>
+        <f t="shared" ref="F3:F20" si="2">D3/B3</f>
         <v>0.96666666666666667</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G20" si="2">(B3-C3)/B3</f>
+        <f t="shared" ref="G3:G20" si="3">(B3-C3)/B3</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="H3" s="25">
-        <f t="shared" ref="H3:H5" si="3">G3*100</f>
+        <f t="shared" ref="H3:H5" si="4">G3*100</f>
         <v>16.666666666666664</v>
       </c>
       <c r="I3" s="1">
-        <f>(B3-D3)/B3</f>
+        <f t="shared" si="0"/>
         <v>3.3333333333333361E-2</v>
       </c>
       <c r="J3" s="6">
-        <f t="shared" ref="J3:J20" si="4">I3*100</f>
+        <f t="shared" ref="J3:J20" si="5">I3*100</f>
         <v>3.3333333333333361</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="25">
+        <f t="shared" ref="K3:K20" si="6">J3/H3</f>
+        <v>0.20000000000000021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>13.7</v>
       </c>
@@ -785,31 +800,35 @@
         <v>11.2</v>
       </c>
       <c r="E4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80000000000000071</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.93333333333333324</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H4" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.666666666666664</v>
       </c>
       <c r="I4" s="1">
-        <f>(B4-D4)/B4</f>
+        <f t="shared" si="0"/>
         <v>6.6666666666666721E-2</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.6666666666666723</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="25">
+        <f t="shared" si="6"/>
+        <v>0.40000000000000041</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>13.7</v>
       </c>
@@ -823,31 +842,35 @@
         <v>10.8</v>
       </c>
       <c r="E5" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1999999999999993</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H5" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.666666666666664</v>
       </c>
       <c r="I5" s="1">
-        <f>(B5-D5)/B5</f>
+        <f t="shared" si="0"/>
         <v>9.9999999999999936E-2</v>
       </c>
       <c r="J5" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.9999999999999929</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="26">
+        <f t="shared" si="6"/>
+        <v>0.59999999999999964</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>23.7</v>
       </c>
@@ -861,15 +884,15 @@
         <v>22</v>
       </c>
       <c r="E6" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15909090909090909</v>
       </c>
       <c r="H6" s="25">
@@ -877,15 +900,19 @@
         <v>15.909090909090908</v>
       </c>
       <c r="I6" s="5">
-        <f>(B6-D6)/B6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J6" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>23.7</v>
       </c>
@@ -899,15 +926,15 @@
         <v>20.5</v>
       </c>
       <c r="E7" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.93181818181818177</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15909090909090909</v>
       </c>
       <c r="H7" s="25">
@@ -915,15 +942,19 @@
         <v>15.909090909090908</v>
       </c>
       <c r="I7" s="1">
-        <f>(B7-D7)/B7</f>
+        <f t="shared" si="0"/>
         <v>6.8181818181818177E-2</v>
       </c>
       <c r="J7" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.8181818181818175</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="25">
+        <f t="shared" si="6"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>23.7</v>
       </c>
@@ -937,15 +968,15 @@
         <v>18.899999999999999</v>
       </c>
       <c r="E8" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1000000000000014</v>
       </c>
       <c r="F8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85909090909090902</v>
       </c>
       <c r="G8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15909090909090909</v>
       </c>
       <c r="H8" s="25">
@@ -953,15 +984,19 @@
         <v>15.909090909090908</v>
       </c>
       <c r="I8" s="10">
-        <f>(B8-D8)/B8</f>
+        <f t="shared" si="0"/>
         <v>0.14090909090909098</v>
       </c>
       <c r="J8" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.090909090909099</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="26">
+        <f t="shared" si="6"/>
+        <v>0.88571428571428623</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>27.7</v>
       </c>
@@ -975,31 +1010,35 @@
         <v>25.7</v>
       </c>
       <c r="E9" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15175097276264587</v>
       </c>
       <c r="H9" s="24">
-        <f t="shared" ref="H9:H20" si="5">G9*100</f>
+        <f t="shared" ref="H9:H20" si="7">G9*100</f>
         <v>15.175097276264587</v>
       </c>
       <c r="I9" s="5">
-        <f>(B9-D9)/B9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>27.7</v>
       </c>
@@ -1013,31 +1052,35 @@
         <v>25</v>
       </c>
       <c r="E10" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.69999999999999929</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.97276264591439687</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15175097276264587</v>
       </c>
       <c r="H10" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>15.175097276264587</v>
       </c>
       <c r="I10" s="1">
-        <f>(B10-D10)/B10</f>
+        <f t="shared" si="0"/>
         <v>2.7237354085603085E-2</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.7237354085603087</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="25">
+        <f t="shared" si="6"/>
+        <v>0.17948717948717938</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>27.7</v>
       </c>
@@ -1051,31 +1094,35 @@
         <v>24.2</v>
       </c>
       <c r="E11" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.94163424124513617</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15175097276264587</v>
       </c>
       <c r="H11" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>15.175097276264587</v>
       </c>
       <c r="I11" s="1">
-        <f>(B11-D11)/B11</f>
+        <f t="shared" si="0"/>
         <v>5.8365758754863814E-2</v>
       </c>
       <c r="J11" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.836575875486381</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="25">
+        <f t="shared" si="6"/>
+        <v>0.38461538461538469</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>27.7</v>
       </c>
@@ -1089,31 +1136,35 @@
         <v>22.6</v>
       </c>
       <c r="E12" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.0999999999999979</v>
       </c>
       <c r="F12" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.87937743190661488</v>
       </c>
       <c r="G12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15175097276264587</v>
       </c>
       <c r="H12" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>15.175097276264587</v>
       </c>
       <c r="I12" s="10">
-        <f>(B12-D12)/B12</f>
+        <f t="shared" si="0"/>
         <v>0.12062256809338513</v>
       </c>
       <c r="J12" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12.062256809338514</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="25">
+        <f t="shared" si="6"/>
+        <v>0.7948717948717946</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>29.7</v>
       </c>
@@ -1127,31 +1178,35 @@
         <v>28.1</v>
       </c>
       <c r="E13" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.16370106761565842</v>
       </c>
       <c r="H13" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>16.370106761565843</v>
       </c>
       <c r="I13" s="1">
-        <f>(B13-D13)/B13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>29.7</v>
       </c>
@@ -1165,31 +1220,35 @@
         <v>26.4</v>
       </c>
       <c r="E14" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7000000000000028</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.93950177935943047</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.16370106761565842</v>
       </c>
       <c r="H14" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>16.370106761565843</v>
       </c>
       <c r="I14" s="1">
-        <f>(B14-D14)/B14</f>
+        <f t="shared" si="0"/>
         <v>6.0498220640569492E-2</v>
       </c>
       <c r="J14" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.0498220640569489</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="25">
+        <f t="shared" si="6"/>
+        <v>0.36956521739130477</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>29.7</v>
       </c>
@@ -1203,31 +1262,35 @@
         <v>25.3</v>
       </c>
       <c r="E15" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8000000000000007</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.90035587188612098</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.16370106761565842</v>
       </c>
       <c r="H15" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>16.370106761565843</v>
       </c>
       <c r="I15" s="1">
-        <f>(B15-D15)/B15</f>
+        <f t="shared" si="0"/>
         <v>9.964412811387903E-2</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.9644128113879038</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="25">
+        <f t="shared" si="6"/>
+        <v>0.60869565217391297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>29.7</v>
       </c>
@@ -1241,31 +1304,35 @@
         <v>24</v>
       </c>
       <c r="E16" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1000000000000014</v>
       </c>
       <c r="F16" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85409252669039137</v>
       </c>
       <c r="G16" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.16370106761565842</v>
       </c>
       <c r="H16" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>16.370106761565843</v>
       </c>
       <c r="I16" s="10">
-        <f>(B16-D16)/B16</f>
+        <f t="shared" si="0"/>
         <v>0.14590747330960857</v>
       </c>
       <c r="J16" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.590747330960857</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="26">
+        <f t="shared" si="6"/>
+        <v>0.89130434782608681</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>30</v>
       </c>
@@ -1279,31 +1346,35 @@
         <v>28.1</v>
       </c>
       <c r="E17" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.14590747330960857</v>
       </c>
       <c r="H17" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>14.590747330960857</v>
       </c>
       <c r="I17" s="1">
-        <f>(B17-D17)/B17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>30</v>
       </c>
@@ -1317,31 +1388,35 @@
         <v>26.9</v>
       </c>
       <c r="E18" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2000000000000028</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95729537366548034</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.14590747330960857</v>
       </c>
       <c r="H18" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>14.590747330960857</v>
       </c>
       <c r="I18" s="1">
-        <f>(B18-D18)/B18</f>
+        <f t="shared" si="0"/>
         <v>4.2704626334519671E-2</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.2704626334519675</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="25">
+        <f t="shared" si="6"/>
+        <v>0.29268292682926894</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>30</v>
       </c>
@@ -1355,31 +1430,35 @@
         <v>25.9</v>
       </c>
       <c r="E19" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2000000000000028</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.9217081850533807</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.14590747330960857</v>
       </c>
       <c r="H19" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>14.590747330960857</v>
       </c>
       <c r="I19" s="1">
-        <f>(B19-D19)/B19</f>
+        <f t="shared" si="0"/>
         <v>7.8291814946619312E-2</v>
       </c>
       <c r="J19" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.8291814946619311</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="25">
+        <f t="shared" si="6"/>
+        <v>0.53658536585365901</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>30</v>
       </c>
@@ -1393,28 +1472,32 @@
         <v>24.8</v>
       </c>
       <c r="E20" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.3000000000000007</v>
       </c>
       <c r="F20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.88256227758007111</v>
       </c>
       <c r="G20" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.14590747330960857</v>
       </c>
       <c r="H20" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>14.590747330960857</v>
       </c>
       <c r="I20" s="10">
-        <f>(B20-D20)/B20</f>
+        <f t="shared" si="0"/>
         <v>0.11743772241992885</v>
       </c>
       <c r="J20" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11.743772241992884</v>
+      </c>
+      <c r="K20" s="26">
+        <f t="shared" si="6"/>
+        <v>0.80487804878048774</v>
       </c>
     </row>
   </sheetData>
@@ -1426,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D9E6C7-C8D1-42F7-A9AB-FC4C9B32771D}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1588,7 @@
         <v>22.448979591836743</v>
       </c>
       <c r="I2" s="5">
-        <f>(B2-D2)/B2</f>
+        <f t="shared" ref="I2:I18" si="0">(B2-D2)/B2</f>
         <v>0</v>
       </c>
       <c r="J2" s="14">
@@ -1527,27 +1610,27 @@
         <v>8.5</v>
       </c>
       <c r="E3" s="18">
-        <f t="shared" ref="E3:E18" si="0">B3-D3</f>
+        <f t="shared" ref="E3:E18" si="1">B3-D3</f>
         <v>1.3000000000000007</v>
       </c>
       <c r="F3" s="7">
-        <f t="shared" ref="F3:F18" si="1">D3/B3</f>
+        <f t="shared" ref="F3:F18" si="2">D3/B3</f>
         <v>0.86734693877551017</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G18" si="2">(B3-C3)/B3</f>
+        <f t="shared" ref="G3:G18" si="3">(B3-C3)/B3</f>
         <v>0.22448979591836743</v>
       </c>
       <c r="H3" s="25">
-        <f t="shared" ref="H3:H18" si="3">G3*100</f>
+        <f t="shared" ref="H3:H18" si="4">G3*100</f>
         <v>22.448979591836743</v>
       </c>
       <c r="I3" s="1">
-        <f>(B3-D3)/B3</f>
+        <f t="shared" si="0"/>
         <v>0.13265306122448986</v>
       </c>
       <c r="J3" s="6">
-        <f t="shared" ref="J3:J18" si="4">I3*100</f>
+        <f t="shared" ref="J3:J18" si="5">I3*100</f>
         <v>13.265306122448987</v>
       </c>
     </row>
@@ -1565,27 +1648,27 @@
         <v>7.8</v>
       </c>
       <c r="E4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0000000000000009</v>
       </c>
       <c r="F4" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.79591836734693866</v>
       </c>
       <c r="G4" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.22448979591836743</v>
       </c>
       <c r="H4" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22.448979591836743</v>
       </c>
       <c r="I4" s="10">
-        <f>(B4-D4)/B4</f>
+        <f t="shared" si="0"/>
         <v>0.20408163265306131</v>
       </c>
       <c r="J4" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.408163265306133</v>
       </c>
     </row>
@@ -1603,27 +1686,27 @@
         <v>12</v>
       </c>
       <c r="E5" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2416666666666667</v>
       </c>
       <c r="H5" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.166666666666671</v>
       </c>
       <c r="I5" s="5">
-        <f>(B5-D5)/B5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J5" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1641,27 +1724,27 @@
         <v>11</v>
       </c>
       <c r="E6" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F6" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2416666666666667</v>
       </c>
       <c r="H6" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.166666666666671</v>
       </c>
       <c r="I6" s="1">
-        <f>(B6-D6)/B6</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="J6" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3333333333333321</v>
       </c>
     </row>
@@ -1679,27 +1762,27 @@
         <v>10</v>
       </c>
       <c r="E7" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="G7" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2416666666666667</v>
       </c>
       <c r="H7" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.166666666666671</v>
       </c>
       <c r="I7" s="10">
-        <f>(B7-D7)/B7</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="J7" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16.666666666666664</v>
       </c>
     </row>
@@ -1717,27 +1800,27 @@
         <v>22.5</v>
       </c>
       <c r="E8" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24444444444444444</v>
       </c>
       <c r="H8" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.444444444444443</v>
       </c>
       <c r="I8" s="5">
-        <f>(B8-D8)/B8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1755,27 +1838,27 @@
         <v>21.9</v>
       </c>
       <c r="E9" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.97333333333333327</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24444444444444444</v>
       </c>
       <c r="H9" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.444444444444443</v>
       </c>
       <c r="I9" s="1">
-        <f>(B9-D9)/B9</f>
+        <f t="shared" si="0"/>
         <v>2.6666666666666731E-2</v>
       </c>
       <c r="J9" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6666666666666732</v>
       </c>
     </row>
@@ -1793,27 +1876,27 @@
         <v>20.9</v>
       </c>
       <c r="E10" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6000000000000014</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92888888888888888</v>
       </c>
       <c r="G10" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24444444444444444</v>
       </c>
       <c r="H10" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.444444444444443</v>
       </c>
       <c r="I10" s="10">
-        <f>(B10-D10)/B10</f>
+        <f t="shared" si="0"/>
         <v>7.111111111111118E-2</v>
       </c>
       <c r="J10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.1111111111111178</v>
       </c>
     </row>
@@ -1831,27 +1914,27 @@
         <v>27.4</v>
       </c>
       <c r="E11" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24452554744525545</v>
       </c>
       <c r="H11" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.452554744525546</v>
       </c>
       <c r="I11" s="5">
-        <f>(B11-D11)/B11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1869,27 +1952,27 @@
         <v>26.1</v>
       </c>
       <c r="E12" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2999999999999972</v>
       </c>
       <c r="F12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95255474452554756</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24452554744525545</v>
       </c>
       <c r="H12" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.452554744525546</v>
       </c>
       <c r="I12" s="1">
-        <f>(B12-D12)/B12</f>
+        <f t="shared" si="0"/>
         <v>4.7445255474452455E-2</v>
       </c>
       <c r="J12" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.7445255474452459</v>
       </c>
     </row>
@@ -1907,27 +1990,27 @@
         <v>25.2</v>
       </c>
       <c r="E13" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1999999999999993</v>
       </c>
       <c r="F13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.91970802919708028</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24452554744525545</v>
       </c>
       <c r="H13" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.452554744525546</v>
       </c>
       <c r="I13" s="1">
-        <f>(B13-D13)/B13</f>
+        <f t="shared" si="0"/>
         <v>8.0291970802919679E-2</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.0291970802919685</v>
       </c>
     </row>
@@ -1945,27 +2028,27 @@
         <v>24.1</v>
       </c>
       <c r="E14" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2999999999999972</v>
       </c>
       <c r="F14" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.87956204379562053</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24452554744525545</v>
       </c>
       <c r="H14" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.452554744525546</v>
       </c>
       <c r="I14" s="1">
-        <f>(B14-D14)/B14</f>
+        <f t="shared" si="0"/>
         <v>0.12043795620437947</v>
       </c>
       <c r="J14" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12.043795620437947</v>
       </c>
     </row>
@@ -1983,27 +2066,27 @@
         <v>39.799999999999997</v>
       </c>
       <c r="E15" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24874371859296482</v>
       </c>
       <c r="H15" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.874371859296481</v>
       </c>
       <c r="I15" s="5">
-        <f>(B15-D15)/B15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J15" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2021,27 +2104,27 @@
         <v>36.200000000000003</v>
       </c>
       <c r="E16" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.5999999999999943</v>
       </c>
       <c r="F16" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.9095477386934675</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24874371859296482</v>
       </c>
       <c r="H16" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.874371859296481</v>
       </c>
       <c r="I16" s="1">
-        <f>(B16-D16)/B16</f>
+        <f t="shared" si="0"/>
         <v>9.0452261306532528E-2</v>
       </c>
       <c r="J16" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.0452261306532531</v>
       </c>
     </row>
@@ -2059,27 +2142,27 @@
         <v>35.1</v>
       </c>
       <c r="E17" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.6999999999999957</v>
       </c>
       <c r="F17" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.88190954773869357</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24874371859296482</v>
       </c>
       <c r="H17" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.874371859296481</v>
       </c>
       <c r="I17" s="1">
-        <f>(B17-D17)/B17</f>
+        <f t="shared" si="0"/>
         <v>0.11809045226130643</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11.809045226130642</v>
       </c>
     </row>
@@ -2097,27 +2180,27 @@
         <v>32.799999999999997</v>
       </c>
       <c r="E18" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F18" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.82412060301507539</v>
       </c>
       <c r="G18" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24874371859296482</v>
       </c>
       <c r="H18" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.874371859296481</v>
       </c>
       <c r="I18" s="10">
-        <f>(B18-D18)/B18</f>
+        <f t="shared" si="0"/>
         <v>0.17587939698492464</v>
       </c>
       <c r="J18" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.587939698492463</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated P/DP timing and 40mm strain measurements
</commit_message>
<xml_diff>
--- a/DataCollection/BPAparameters_normalized.xlsx
+++ b/DataCollection/BPAparameters_normalized.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB98E2A-0446-42C6-BE3A-15D5B65DBFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F6847F-59B1-4C18-88B7-B53EEBB0EE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{8A3A5EB0-BE78-4EAA-84C9-DD014A3A2FAA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{8A3A5EB0-BE78-4EAA-84C9-DD014A3A2FAA}"/>
   </bookViews>
   <sheets>
     <sheet name="10mm" sheetId="1" r:id="rId1"/>
     <sheet name="20mm" sheetId="2" r:id="rId2"/>
+    <sheet name="40mm" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>Cut length</t>
   </si>
@@ -101,15 +102,34 @@
   <si>
     <t>40cm</t>
   </si>
+  <si>
+    <t>BPA ID (40mm)</t>
+  </si>
+  <si>
+    <t>25cm</t>
+  </si>
+  <si>
+    <t>15cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: Min contraction length is measured at 500kpa due to leaks. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -289,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1556,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D9E6C7-C8D1-42F7-A9AB-FC4C9B32771D}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2271,4 +2292,556 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C12A74-AD6F-4A13-BFF1-649CA085888F}">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4">
+        <v>14.8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>11.5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="4">
+        <f>E2/C2</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <f>(C2-D2)/C2</f>
+        <v>0.27826086956521734</v>
+      </c>
+      <c r="I2" s="24">
+        <f>H2*100</f>
+        <v>27.826086956521735</v>
+      </c>
+      <c r="J2" s="5">
+        <f t="shared" ref="J2:J18" si="0">(C2-E2)/C2</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="14">
+        <f>J2*100</f>
+        <v>100</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="7"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="7" t="e">
+        <f t="shared" ref="G3:G18" si="1">E3/C3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H3" s="1" t="e">
+        <f t="shared" ref="H3:H18" si="2">(C3-D3)/C3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3" s="25" t="e">
+        <f t="shared" ref="I3:I18" si="3">H3*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="6" t="e">
+        <f t="shared" ref="K3:K18" si="4">J3*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L3" s="27"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I4" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="12" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" s="5" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5" s="24" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" s="14" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I6" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="16"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="12" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4">
+        <v>25.2</v>
+      </c>
+      <c r="C8" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="2"/>
+        <v>0.27477477477477469</v>
+      </c>
+      <c r="I8" s="24">
+        <f t="shared" si="3"/>
+        <v>27.477477477477468</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="14">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="12" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="7">
+        <v>29.5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>26.4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" si="2"/>
+        <v>0.27651515151515144</v>
+      </c>
+      <c r="I11" s="24">
+        <f t="shared" si="3"/>
+        <v>27.651515151515145</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K12" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K13" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K14" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="5" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="14" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K16" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K18" s="12" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Optimization Code - Update
save parameters in a matrix for each optimization run (Specified length, and test number) - All kinks and P/DP
</commit_message>
<xml_diff>
--- a/DataCollection/BPAparameters_normalized.xlsx
+++ b/DataCollection/BPAparameters_normalized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F6847F-59B1-4C18-88B7-B53EEBB0EE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F0CAE7-CD56-48F6-B828-CF995D120EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{8A3A5EB0-BE78-4EAA-84C9-DD014A3A2FAA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8A3A5EB0-BE78-4EAA-84C9-DD014A3A2FAA}"/>
   </bookViews>
   <sheets>
     <sheet name="10mm" sheetId="1" r:id="rId1"/>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F760E8-92D5-4163-ADDE-07026F3D9A53}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +709,8 @@
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -1578,7 +1579,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,8 +2299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C12A74-AD6F-4A13-BFF1-649CA085888F}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,6 +2311,7 @@
     <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>